<commit_message>
Caculate C, D, T and plot data
</commit_message>
<xml_diff>
--- a/Document/Other/TKHTN.xlsx
+++ b/Document/Other/TKHTN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TKHTN\TKHTN_2024\TKHTN2024\Document\Other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E41E29A0-B541-4705-9BEF-55FEB5127C0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A21FA8EB-5739-4350-8376-27ED84641558}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="24" yWindow="24" windowWidth="23016" windowHeight="12216" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -407,7 +407,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -427,7 +427,7 @@
       <c r="C2" s="10"/>
       <c r="D2" s="10"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A3" s="10"/>
       <c r="B3" s="10"/>
       <c r="C3" s="9" t="s">
@@ -437,7 +437,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A4" s="10"/>
       <c r="B4" s="9" t="s">
         <v>4</v>
@@ -445,7 +445,7 @@
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A5" s="10"/>
       <c r="B5" s="10"/>
       <c r="C5" s="9" t="s">
@@ -459,7 +459,7 @@
       <c r="C6" s="10"/>
       <c r="D6" s="10"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>6</v>
       </c>
@@ -469,7 +469,7 @@
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A8" s="10"/>
       <c r="B8" s="1" t="s">
         <v>8</v>
@@ -506,7 +506,7 @@
   <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -564,7 +564,7 @@
       </c>
       <c r="G2" s="4"/>
       <c r="H2" s="4">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="I2" s="6" t="s">
         <v>13</v>
@@ -596,7 +596,7 @@
         <v>0</v>
       </c>
       <c r="H3" s="4">
-        <v>481</v>
+        <v>494</v>
       </c>
       <c r="I3" s="6" t="s">
         <v>14</v>
@@ -628,7 +628,7 @@
         <v>1</v>
       </c>
       <c r="H4" s="4">
-        <v>481</v>
+        <v>494</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -654,7 +654,7 @@
         <v>2</v>
       </c>
       <c r="H5" s="4">
-        <v>481</v>
+        <v>494</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -680,7 +680,7 @@
         <v>3</v>
       </c>
       <c r="H6" s="4">
-        <v>481</v>
+        <v>494</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -706,7 +706,7 @@
         <v>4</v>
       </c>
       <c r="H7" s="4">
-        <v>481</v>
+        <v>494</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -732,7 +732,7 @@
         <v>5</v>
       </c>
       <c r="H8" s="4">
-        <v>481</v>
+        <v>494</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -758,7 +758,7 @@
         <v>6</v>
       </c>
       <c r="H9" s="4">
-        <v>481</v>
+        <v>494</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -784,7 +784,7 @@
         <v>7</v>
       </c>
       <c r="H10" s="4">
-        <v>481</v>
+        <v>494</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -810,7 +810,7 @@
         <v>8</v>
       </c>
       <c r="H11" s="4">
-        <v>481</v>
+        <v>494</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -836,7 +836,7 @@
         <v>9</v>
       </c>
       <c r="H12" s="4">
-        <v>481</v>
+        <v>494</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -862,7 +862,7 @@
         <v>15</v>
       </c>
       <c r="H13" s="4">
-        <v>481</v>
+        <v>499</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -888,7 +888,7 @@
         <v>16</v>
       </c>
       <c r="H14" s="4">
-        <v>481</v>
+        <v>735</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>